<commit_message>
production for each material in the same sheets
</commit_message>
<xml_diff>
--- a/test_usgs/trash/sub_materials_database.xlsx
+++ b/test_usgs/trash/sub_materials_database.xlsx
@@ -119,10 +119,10 @@
     <t>n thousand metric dry tons</t>
   </si>
   <si>
-    <t>sub_material_name</t>
-  </si>
-  <si>
-    <t>chemical_composition</t>
+    <t>Sub Material Name</t>
+  </si>
+  <si>
+    <t>Chemical Composition</t>
   </si>
   <si>
     <t>Fused Aluminum Oxide</t>

</xml_diff>